<commit_message>
map data for BangKeSuDungTienVay + DonCamKet
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/bidv/SampleData/HOÁ ĐƠN.xlsx
+++ b/adg-api/src/main/resources/bidv/SampleData/HOÁ ĐƠN.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-api/src/main/resources/bidv/SampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7F9C28-403A-4F45-9A7D-968A05E00946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A948427-5AE0-1A49-B2C5-87EAB6E1FC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="4060" windowWidth="36600" windowHeight="21140" xr2:uid="{A243C796-5D2C-5240-850F-FA3C1FE3FD22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -569,11 +570,13 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="5" max="5" width="45.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
     <col min="15" max="16" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
map data for BienBanKiemTraSuDungVonVay
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/bidv/SampleData/HOÁ ĐƠN.xlsx
+++ b/adg-api/src/main/resources/bidv/SampleData/HOÁ ĐƠN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-api/src/main/resources/bidv/SampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A948427-5AE0-1A49-B2C5-87EAB6E1FC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB66DFA3-8121-E949-8D76-9368F110F89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="4060" windowWidth="36600" windowHeight="21140" xr2:uid="{A243C796-5D2C-5240-850F-FA3C1FE3FD22}"/>
   </bookViews>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B26698-F151-B841-90E8-9BD5F17B6B5E}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>